<commit_message>
Fixed in Greenbook everything except military construction.
</commit_message>
<xml_diff>
--- a/Output/Greenbook.xlsx
+++ b/Output/Greenbook.xlsx
@@ -15,15 +15,15 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Greenbook" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="22" r:id="rId3"/>
+    <pivotCache cacheId="27" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="17">
   <si>
     <t>OMBbureau</t>
   </si>
@@ -82,7 +82,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -574,8 +574,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -624,28 +624,28 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,9 +661,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="gsand_000" refreshedDate="42828.167743865743" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="28">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="gsand_000" refreshedDate="42828.192631134261" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="33">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B1:F29" sheet="Greenbook"/>
+    <worksheetSource ref="B1:F34" sheet="Greenbook"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="OMBbureau" numFmtId="0">
@@ -679,21 +679,21 @@
     <cacheField name="SourceFiscalYear" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2012" maxValue="2017" count="6">
         <n v="2012"/>
+        <n v="2013"/>
         <n v="2014"/>
         <n v="2015"/>
         <n v="2016"/>
         <n v="2017"/>
-        <n v="2013"/>
       </sharedItems>
     </cacheField>
     <cacheField name="FiscalYear" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2011" maxValue="2016" count="6">
         <n v="2011"/>
+        <n v="2012"/>
         <n v="2013"/>
         <n v="2014"/>
         <n v="2015"/>
         <n v="2016"/>
-        <n v="2012"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Base" numFmtId="0">
@@ -712,7 +712,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="28">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="33">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -724,27 +724,34 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <n v="139918046"/>
-    <n v="14060094"/>
+    <n v="141818404"/>
+    <n v="11293469"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
-    <n v="135911527"/>
-    <n v="8149300"/>
+    <n v="139918046"/>
+    <n v="14060094"/>
   </r>
   <r>
     <x v="0"/>
     <x v="3"/>
     <x v="3"/>
-    <n v="134962072"/>
-    <n v="5031927"/>
+    <n v="135911527"/>
+    <n v="8149300"/>
   </r>
   <r>
     <x v="0"/>
     <x v="4"/>
     <x v="4"/>
+    <n v="134962072"/>
+    <n v="5031927"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
     <n v="135330213"/>
     <n v="3222673"/>
   </r>
@@ -759,27 +766,34 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <n v="199169928"/>
-    <n v="63986203"/>
+    <n v="197871987"/>
+    <n v="87132652"/>
   </r>
   <r>
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <n v="195263995"/>
-    <n v="69682894"/>
+    <n v="199169928"/>
+    <n v="63986203"/>
   </r>
   <r>
     <x v="1"/>
     <x v="3"/>
     <x v="3"/>
-    <n v="195487638"/>
-    <n v="51745357"/>
+    <n v="195263995"/>
+    <n v="69682894"/>
   </r>
   <r>
     <x v="1"/>
     <x v="4"/>
     <x v="4"/>
+    <n v="195487638"/>
+    <n v="51745357"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="5"/>
     <n v="198530109"/>
     <n v="46472636"/>
   </r>
@@ -794,27 +808,34 @@
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <n v="2716103"/>
-    <n v="503364"/>
+    <n v="2640085"/>
+    <n v="435013"/>
   </r>
   <r>
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <n v="2246427"/>
-    <n v="264910"/>
+    <n v="2716103"/>
+    <n v="503364"/>
   </r>
   <r>
     <x v="2"/>
     <x v="3"/>
     <x v="3"/>
-    <n v="2134480"/>
-    <n v="91350"/>
+    <n v="2246427"/>
+    <n v="264910"/>
   </r>
   <r>
     <x v="2"/>
     <x v="4"/>
     <x v="4"/>
+    <n v="2134480"/>
+    <n v="91350"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="5"/>
     <n v="2212932"/>
     <n v="88850"/>
   </r>
@@ -829,27 +850,34 @@
     <x v="3"/>
     <x v="1"/>
     <x v="1"/>
-    <n v="105889212"/>
-    <n v="9587241"/>
+    <n v="106132202"/>
+    <n v="16075445"/>
   </r>
   <r>
     <x v="3"/>
     <x v="2"/>
     <x v="2"/>
-    <n v="93676482"/>
-    <n v="7112381"/>
+    <n v="105889212"/>
+    <n v="9587241"/>
   </r>
   <r>
     <x v="3"/>
     <x v="3"/>
     <x v="3"/>
-    <n v="94821073"/>
-    <n v="8158155"/>
+    <n v="93676482"/>
+    <n v="7112381"/>
   </r>
   <r>
     <x v="3"/>
     <x v="4"/>
     <x v="4"/>
+    <n v="94821073"/>
+    <n v="8158155"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
     <n v="117481331"/>
     <n v="8128888"/>
   </r>
@@ -864,27 +892,34 @@
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
-    <n v="74116081"/>
-    <n v="245516"/>
+    <n v="74036863"/>
+    <n v="526358"/>
   </r>
   <r>
     <x v="4"/>
     <x v="2"/>
     <x v="2"/>
-    <n v="65196138"/>
-    <n v="135134"/>
+    <n v="74116081"/>
+    <n v="245516"/>
   </r>
   <r>
     <x v="4"/>
     <x v="3"/>
     <x v="3"/>
-    <n v="66036426"/>
-    <n v="322373"/>
+    <n v="65196138"/>
+    <n v="135134"/>
   </r>
   <r>
     <x v="4"/>
     <x v="4"/>
     <x v="4"/>
+    <n v="66036426"/>
+    <n v="322373"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="5"/>
     <n v="72465107"/>
     <n v="231434"/>
   </r>
@@ -897,15 +932,15 @@
   </r>
   <r>
     <x v="5"/>
-    <x v="5"/>
-    <x v="5"/>
+    <x v="1"/>
+    <x v="1"/>
     <n v="53981540"/>
     <n v="988424"/>
   </r>
   <r>
     <x v="5"/>
-    <x v="3"/>
-    <x v="3"/>
+    <x v="4"/>
+    <x v="4"/>
     <n v="25315193"/>
     <n v="867560"/>
   </r>
@@ -913,8 +948,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C44" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C49" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
@@ -930,22 +965,22 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item x="0"/>
-        <item x="5"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item x="0"/>
-        <item x="5"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -957,7 +992,7 @@
     <field x="2"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="41">
+  <rowItems count="46">
     <i>
       <x/>
     </i>
@@ -990,6 +1025,21 @@
     </i>
     <i r="2">
       <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
     </i>
     <i>
       <x v="2"/>
@@ -1431,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G44"/>
+  <dimension ref="A3:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,10 +1598,10 @@
         <v>2013</v>
       </c>
       <c r="B12" s="6">
-        <v>53981540</v>
+        <v>576481081</v>
       </c>
       <c r="C12" s="6">
-        <v>988424</v>
+        <v>116451361</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1559,10 +1609,10 @@
         <v>2012</v>
       </c>
       <c r="B13" s="6">
-        <v>53981540</v>
+        <v>576481081</v>
       </c>
       <c r="C13" s="6">
-        <v>988424</v>
+        <v>116451361</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1577,36 +1627,36 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2014</v>
+      <c r="A15" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B15" s="6">
-        <v>521809370</v>
+        <v>141818404</v>
       </c>
       <c r="C15" s="6">
-        <v>88382418</v>
+        <v>11293469</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>2013</v>
+      <c r="A16" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B16" s="6">
-        <v>521809370</v>
+        <v>197871987</v>
       </c>
       <c r="C16" s="6">
-        <v>88382418</v>
+        <v>87132652</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B17" s="6">
-        <v>139918046</v>
+        <v>106132202</v>
       </c>
       <c r="C17" s="6">
-        <v>14060094</v>
+        <v>16075445</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
@@ -1614,13 +1664,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B18" s="6">
-        <v>199169928</v>
+        <v>74036863</v>
       </c>
       <c r="C18" s="6">
-        <v>63986203</v>
+        <v>526358</v>
       </c>
       <c r="E18">
         <v>2014</v>
@@ -1634,288 +1684,343 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="6">
-        <v>105889212</v>
+        <v>2640085</v>
       </c>
       <c r="C19" s="6">
-        <v>9587241</v>
+        <v>435013</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>9</v>
+      <c r="A20" s="2">
+        <v>2014</v>
       </c>
       <c r="B20" s="6">
-        <v>74116081</v>
+        <v>521809370</v>
       </c>
       <c r="C20" s="6">
-        <v>245516</v>
+        <v>88382418</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>7</v>
+      <c r="A21" s="3">
+        <v>2013</v>
       </c>
       <c r="B21" s="6">
-        <v>2716103</v>
+        <v>521809370</v>
       </c>
       <c r="C21" s="6">
-        <v>503364</v>
+        <v>88382418</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>2015</v>
+      <c r="A22" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B22" s="6">
-        <v>492294569</v>
+        <v>139918046</v>
       </c>
       <c r="C22" s="6">
-        <v>85344619</v>
+        <v>14060094</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>2014</v>
+      <c r="A23" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B23" s="6">
-        <v>492294569</v>
+        <v>199169928</v>
       </c>
       <c r="C23" s="6">
-        <v>85344619</v>
+        <v>63986203</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B24" s="6">
-        <v>135911527</v>
+        <v>105889212</v>
       </c>
       <c r="C24" s="6">
-        <v>8149300</v>
+        <v>9587241</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B25" s="6">
-        <v>195263995</v>
+        <v>74116081</v>
       </c>
       <c r="C25" s="6">
-        <v>69682894</v>
+        <v>245516</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" s="6">
-        <v>93676482</v>
+        <v>2716103</v>
       </c>
       <c r="C26" s="6">
-        <v>7112381</v>
+        <v>503364</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>9</v>
+      <c r="A27" s="2">
+        <v>2015</v>
       </c>
       <c r="B27" s="6">
-        <v>65196138</v>
+        <v>492294569</v>
       </c>
       <c r="C27" s="6">
-        <v>135134</v>
+        <v>85344619</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>7</v>
+      <c r="A28" s="3">
+        <v>2014</v>
       </c>
       <c r="B28" s="6">
-        <v>2246427</v>
+        <v>492294569</v>
       </c>
       <c r="C28" s="6">
-        <v>264910</v>
+        <v>85344619</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>2016</v>
+      <c r="A29" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B29" s="6">
-        <v>518756882</v>
+        <v>135911527</v>
       </c>
       <c r="C29" s="6">
-        <v>66216722</v>
+        <v>8149300</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>2015</v>
+      <c r="A30" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B30" s="6">
-        <v>518756882</v>
+        <v>195263995</v>
       </c>
       <c r="C30" s="6">
-        <v>66216722</v>
+        <v>69682894</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31" s="6">
-        <v>25315193</v>
+        <v>93676482</v>
       </c>
       <c r="C31" s="6">
-        <v>867560</v>
+        <v>7112381</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B32" s="6">
-        <v>134962072</v>
+        <v>65196138</v>
       </c>
       <c r="C32" s="6">
-        <v>5031927</v>
+        <v>135134</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B33" s="6">
-        <v>195487638</v>
+        <v>2246427</v>
       </c>
       <c r="C33" s="6">
-        <v>51745357</v>
+        <v>264910</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>8</v>
+      <c r="A34" s="2">
+        <v>2016</v>
       </c>
       <c r="B34" s="6">
-        <v>94821073</v>
+        <v>518756882</v>
       </c>
       <c r="C34" s="6">
-        <v>8158155</v>
+        <v>66216722</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>9</v>
+      <c r="A35" s="3">
+        <v>2015</v>
       </c>
       <c r="B35" s="6">
-        <v>66036426</v>
+        <v>518756882</v>
       </c>
       <c r="C35" s="6">
-        <v>322373</v>
+        <v>66216722</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B36" s="6">
-        <v>2134480</v>
+        <v>25315193</v>
       </c>
       <c r="C36" s="6">
-        <v>91350</v>
+        <v>867560</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>2017</v>
+      <c r="A37" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B37" s="6">
-        <v>526019692</v>
+        <v>134962072</v>
       </c>
       <c r="C37" s="6">
-        <v>58144481</v>
+        <v>5031927</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>2016</v>
+      <c r="A38" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B38" s="6">
-        <v>526019692</v>
+        <v>195487638</v>
       </c>
       <c r="C38" s="6">
-        <v>58144481</v>
+        <v>51745357</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B39" s="6">
-        <v>135330213</v>
+        <v>94821073</v>
       </c>
       <c r="C39" s="6">
-        <v>3222673</v>
+        <v>8158155</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B40" s="6">
-        <v>198530109</v>
+        <v>66036426</v>
       </c>
       <c r="C40" s="6">
-        <v>46472636</v>
+        <v>322373</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="6">
+        <v>2134480</v>
+      </c>
+      <c r="C41" s="6">
+        <v>91350</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B42" s="6">
+        <v>526019692</v>
+      </c>
+      <c r="C42" s="6">
+        <v>58144481</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>2016</v>
+      </c>
+      <c r="B43" s="6">
+        <v>526019692</v>
+      </c>
+      <c r="C43" s="6">
+        <v>58144481</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="6">
+        <v>135330213</v>
+      </c>
+      <c r="C44" s="6">
+        <v>3222673</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="6">
+        <v>198530109</v>
+      </c>
+      <c r="C45" s="6">
+        <v>46472636</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B46" s="6">
         <v>117481331</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C46" s="6">
         <v>8128888</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B47" s="6">
         <v>72465107</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C47" s="6">
         <v>231434</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B48" s="6">
         <v>2212932</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C48" s="6">
         <v>88850</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="6">
-        <v>2728188767</v>
-      </c>
-      <c r="C44" s="6">
-        <v>464526795</v>
+      <c r="B49" s="6">
+        <v>3250688308</v>
+      </c>
+      <c r="C49" s="6">
+        <v>579989732</v>
       </c>
     </row>
   </sheetData>
@@ -1925,10 +2030,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection sqref="A1:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,16 +2083,16 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D3">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="E3">
-        <v>139918046</v>
+        <v>141818404</v>
       </c>
       <c r="F3">
-        <v>14060094</v>
+        <v>11293469</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1998,16 +2103,16 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D4">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="E4">
-        <v>135911527</v>
+        <v>139918046</v>
       </c>
       <c r="F4">
-        <v>8149300</v>
+        <v>14060094</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2018,16 +2123,16 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D5">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="E5">
-        <v>134962072</v>
+        <v>135911527</v>
       </c>
       <c r="F5">
-        <v>5031927</v>
+        <v>8149300</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2038,16 +2143,16 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D6">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E6">
-        <v>135330213</v>
+        <v>134962072</v>
       </c>
       <c r="F6">
-        <v>3222673</v>
+        <v>5031927</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2055,19 +2160,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="D7">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="E7">
-        <v>184960729</v>
+        <v>135330213</v>
       </c>
       <c r="F7">
-        <v>109648488</v>
+        <v>3222673</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2078,16 +2183,16 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D8">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="E8">
-        <v>199169928</v>
+        <v>184960729</v>
       </c>
       <c r="F8">
-        <v>63986203</v>
+        <v>109648488</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2098,16 +2203,16 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D9">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="E9">
-        <v>195263995</v>
+        <v>197871987</v>
       </c>
       <c r="F9">
-        <v>69682894</v>
+        <v>87132652</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2118,16 +2223,16 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D10">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E10">
-        <v>195487638</v>
+        <v>199169928</v>
       </c>
       <c r="F10">
-        <v>51745357</v>
+        <v>63986203</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2138,16 +2243,16 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="D11">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="E11">
-        <v>198530109</v>
+        <v>195263995</v>
       </c>
       <c r="F11">
-        <v>46472636</v>
+        <v>69682894</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2155,19 +2260,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="D12">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="E12">
-        <v>3118762</v>
+        <v>195487638</v>
       </c>
       <c r="F12">
-        <v>1449436</v>
+        <v>51745357</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2175,19 +2280,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="D13">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="E13">
-        <v>2716103</v>
+        <v>198530109</v>
       </c>
       <c r="F13">
-        <v>503364</v>
+        <v>46472636</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,16 +2303,16 @@
         <v>7</v>
       </c>
       <c r="C14">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="D14">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="E14">
-        <v>2246427</v>
+        <v>3118762</v>
       </c>
       <c r="F14">
-        <v>264910</v>
+        <v>1449436</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2218,16 +2323,16 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="D15">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="E15">
-        <v>2134480</v>
+        <v>2640085</v>
       </c>
       <c r="F15">
-        <v>91350</v>
+        <v>435013</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2238,16 +2343,16 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="D16">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="E16">
-        <v>2212932</v>
+        <v>2716103</v>
       </c>
       <c r="F16">
-        <v>88850</v>
+        <v>503364</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2255,19 +2360,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="D17">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="E17">
-        <v>104789161</v>
+        <v>2246427</v>
       </c>
       <c r="F17">
-        <v>29374960</v>
+        <v>264910</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2275,19 +2380,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="D18">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="E18">
-        <v>105889212</v>
+        <v>2134480</v>
       </c>
       <c r="F18">
-        <v>9587241</v>
+        <v>91350</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2295,19 +2400,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="D19">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E19">
-        <v>93676482</v>
+        <v>2212932</v>
       </c>
       <c r="F19">
-        <v>7112381</v>
+        <v>88850</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2318,16 +2423,16 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="D20">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="E20">
-        <v>94821073</v>
+        <v>104789161</v>
       </c>
       <c r="F20">
-        <v>8158155</v>
+        <v>29374960</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,16 +2443,16 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="D21">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="E21">
-        <v>117481331</v>
+        <v>106132202</v>
       </c>
       <c r="F21">
-        <v>8128888</v>
+        <v>16075445</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,19 +2460,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="D22">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="E22">
-        <v>81307939</v>
+        <v>105889212</v>
       </c>
       <c r="F22">
-        <v>518294</v>
+        <v>9587241</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2375,19 +2480,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23">
+        <v>2015</v>
+      </c>
+      <c r="D23">
         <v>2014</v>
       </c>
-      <c r="D23">
-        <v>2013</v>
-      </c>
       <c r="E23">
-        <v>74116081</v>
+        <v>93676482</v>
       </c>
       <c r="F23">
-        <v>245516</v>
+        <v>7112381</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2395,19 +2500,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24">
+        <v>2016</v>
+      </c>
+      <c r="D24">
         <v>2015</v>
       </c>
-      <c r="D24">
-        <v>2014</v>
-      </c>
       <c r="E24">
-        <v>65196138</v>
+        <v>94821073</v>
       </c>
       <c r="F24">
-        <v>135134</v>
+        <v>8158155</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2415,19 +2520,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25">
+        <v>2017</v>
+      </c>
+      <c r="D25">
         <v>2016</v>
       </c>
-      <c r="D25">
-        <v>2015</v>
-      </c>
       <c r="E25">
-        <v>66036426</v>
+        <v>117481331</v>
       </c>
       <c r="F25">
-        <v>322373</v>
+        <v>8128888</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2438,16 +2543,16 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="D26">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="E26">
-        <v>72465107</v>
+        <v>81307939</v>
       </c>
       <c r="F26">
-        <v>231434</v>
+        <v>518294</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2455,19 +2560,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27">
+        <v>2013</v>
+      </c>
+      <c r="D27">
         <v>2012</v>
       </c>
-      <c r="D27">
-        <v>2011</v>
-      </c>
       <c r="E27">
-        <v>105969085</v>
+        <v>74036863</v>
       </c>
       <c r="F27">
-        <v>7815988</v>
+        <v>526358</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2475,19 +2580,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28">
+        <v>2014</v>
+      </c>
+      <c r="D28">
         <v>2013</v>
       </c>
-      <c r="D28">
-        <v>2012</v>
-      </c>
       <c r="E28">
-        <v>53981540</v>
+        <v>74116081</v>
       </c>
       <c r="F28">
-        <v>988424</v>
+        <v>245516</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2495,18 +2600,118 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>2015</v>
+      </c>
+      <c r="D29">
+        <v>2014</v>
+      </c>
+      <c r="E29">
+        <v>65196138</v>
+      </c>
+      <c r="F29">
+        <v>135134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>2016</v>
+      </c>
+      <c r="D30">
+        <v>2015</v>
+      </c>
+      <c r="E30">
+        <v>66036426</v>
+      </c>
+      <c r="F30">
+        <v>322373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>2017</v>
+      </c>
+      <c r="D31">
+        <v>2016</v>
+      </c>
+      <c r="E31">
+        <v>72465107</v>
+      </c>
+      <c r="F31">
+        <v>231434</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>10</v>
       </c>
-      <c r="C29">
+      <c r="C32">
+        <v>2012</v>
+      </c>
+      <c r="D32">
+        <v>2011</v>
+      </c>
+      <c r="E32">
+        <v>105969085</v>
+      </c>
+      <c r="F32">
+        <v>7815988</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>2013</v>
+      </c>
+      <c r="D33">
+        <v>2012</v>
+      </c>
+      <c r="E33">
+        <v>53981540</v>
+      </c>
+      <c r="F33">
+        <v>988424</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
         <v>2016</v>
       </c>
-      <c r="D29">
+      <c r="D34">
         <v>2015</v>
       </c>
-      <c r="E29">
+      <c r="E34">
         <v>25315193</v>
       </c>
-      <c r="F29">
+      <c r="F34">
         <v>867560</v>
       </c>
     </row>

</xml_diff>